<commit_message>
Version 1.1.0 - Penyesuaian Template CKP
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\app\khi\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF0DE3A-E714-491A-93D5-2B7D0D71EB8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DADC0D-EE42-4A83-BE7C-B2C5406D2EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="630" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="630" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CKP_R" sheetId="1" r:id="rId1"/>
@@ -145,10 +145,10 @@
     <t>CAPAIAN KINERJA PEGAWAI TAHUN 2025</t>
   </si>
   <si>
-    <t>Aulia Rahman SE, M.Si</t>
-  </si>
-  <si>
-    <t>NIP. 198610062006041008</t>
+    <t>Abdul Razi S.Si</t>
+  </si>
+  <si>
+    <t>NIP. 197612291999011001</t>
   </si>
 </sst>
 </file>
@@ -574,24 +574,42 @@
     <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -609,30 +627,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -643,9 +646,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -929,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -961,19 +961,19 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="19.5" thickTop="1">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1"/>
@@ -1064,39 +1064,39 @@
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="58" t="s">
+      <c r="C9" s="38"/>
+      <c r="D9" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="40"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="58" t="s">
+      <c r="F9" s="49"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="61" t="s">
+      <c r="I9" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="61" t="s">
+      <c r="J9" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="58" t="s">
+      <c r="K9" s="43" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="43"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="43"/>
+      <c r="A10" s="44"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="44"/>
       <c r="E10" s="3" t="s">
         <v>13</v>
       </c>
@@ -1106,20 +1106,20 @@
       <c r="G10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="44"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="4">
         <v>-1</v>
       </c>
-      <c r="B11" s="51">
+      <c r="B11" s="34">
         <f>A11-1</f>
         <v>-2</v>
       </c>
-      <c r="C11" s="41"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="4">
         <f>B11-1</f>
         <v>-3</v>
@@ -1154,11 +1154,11 @@
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="52" t="s">
+      <c r="A12" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="53"/>
-      <c r="C12" s="54"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -1170,8 +1170,8 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="6"/>
-      <c r="B13" s="55"/>
-      <c r="C13" s="56"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="40"/>
       <c r="D13" s="6"/>
       <c r="E13" s="7"/>
       <c r="F13" s="6"/>
@@ -1182,11 +1182,11 @@
       <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="47"/>
-      <c r="C14" s="48"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="56"/>
       <c r="D14" s="10"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -1200,8 +1200,8 @@
       <c r="A15" s="13">
         <v>1</v>
       </c>
-      <c r="B15" s="49"/>
-      <c r="C15" s="50"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="58"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
@@ -1212,17 +1212,17 @@
       <c r="K15" s="16"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="38"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="47"/>
       <c r="J16" s="17">
         <f>SUM(J12:J13)</f>
         <v>0</v>
@@ -1230,14 +1230,14 @@
       <c r="K16" s="18"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="41"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="35"/>
       <c r="G17" s="19" t="e">
         <f>AVERAGE(G13:G15)</f>
         <v>#DIV/0!</v>
@@ -1249,26 +1249,26 @@
       <c r="I17" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="42"/>
-      <c r="K17" s="44"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="52"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="45" t="e">
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="53" t="e">
         <f>AVERAGE(G17:H17)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H18" s="41"/>
+      <c r="H18" s="35"/>
       <c r="I18" s="17"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="43"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="44"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="21"/>
@@ -1335,10 +1335,10 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="34" t="s">
+      <c r="G23" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="H23" s="35"/>
+      <c r="H23" s="42"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -1363,10 +1363,10 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="34" t="s">
+      <c r="G25" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="H25" s="34"/>
+      <c r="H25" s="59"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -1378,16 +1378,27 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="34" t="s">
+      <c r="G26" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="H26" s="34"/>
+      <c r="H26" s="59"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="A16:I16"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="B15:C15"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="B13:C13"/>
@@ -1400,17 +1411,6 @@
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="K9:K10"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="A16:I16"/>
-    <mergeCell ref="A17:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -1421,8 +1421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D651DB4-1B97-40CF-840B-915296A88124}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23:G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1446,16 +1446,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="19.5" thickTop="1">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1"/>
@@ -1528,48 +1528,48 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="63" t="s">
+      <c r="C9" s="38"/>
+      <c r="D9" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="65" t="s">
+      <c r="E9" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="65" t="s">
+      <c r="F9" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="65" t="s">
+      <c r="G9" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="63" t="s">
+      <c r="H9" s="64" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="43"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
+      <c r="A10" s="44"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="4">
         <v>-1</v>
       </c>
-      <c r="B11" s="51">
+      <c r="B11" s="34">
         <f>A11-1</f>
         <v>-2</v>
       </c>
-      <c r="C11" s="41"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="4">
         <f>B11-1</f>
         <v>-3</v>
@@ -1592,11 +1592,11 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="52" t="s">
+      <c r="A12" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="53"/>
-      <c r="C12" s="54"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -1607,8 +1607,8 @@
       <c r="A13" s="6">
         <v>1</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="56"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="40"/>
       <c r="D13" s="6"/>
       <c r="E13" s="7"/>
       <c r="F13" s="6"/>
@@ -1616,11 +1616,11 @@
       <c r="H13" s="25"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="47"/>
-      <c r="C14" s="48"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="56"/>
       <c r="D14" s="10"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -1631,8 +1631,8 @@
       <c r="A15" s="13">
         <v>1</v>
       </c>
-      <c r="B15" s="49"/>
-      <c r="C15" s="50"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="58"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
@@ -1640,14 +1640,14 @@
       <c r="H15" s="27"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="66" t="s">
+      <c r="A16" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="41"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="35"/>
       <c r="G16" s="28">
         <f>SUM(G12:G15)</f>
         <v>0</v>
@@ -1757,8 +1757,8 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="35"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="42"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="21"/>
@@ -1767,16 +1767,11 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="35"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A14:C14"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="B13:C13"/>
@@ -1788,6 +1783,11 @@
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="H9:H10"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A14:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Version 2.1.1 - Update CKP-T Mengikuti Pengisian KHI Bulan Selanjutnya
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\app\khi\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DADC0D-EE42-4A83-BE7C-B2C5406D2EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BA76D7-DB6C-4F41-B652-749CA42997AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="630" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CKP_R" sheetId="1" r:id="rId1"/>
     <sheet name="CKP_T" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">CKP_R!$A$1:$K$26</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">CKP_R!$A$1:$K$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -574,10 +574,44 @@
     <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -590,53 +624,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -646,6 +643,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -929,7 +929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -961,19 +961,19 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="19.5" thickTop="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1"/>
@@ -1064,39 +1064,39 @@
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="43" t="s">
+      <c r="C9" s="54"/>
+      <c r="D9" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="48" t="s">
+      <c r="E9" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="49"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="43" t="s">
+      <c r="F9" s="40"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="50" t="s">
+      <c r="I9" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="50" t="s">
+      <c r="J9" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="43" t="s">
+      <c r="K9" s="58" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="44"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="44"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="43"/>
       <c r="E10" s="3" t="s">
         <v>13</v>
       </c>
@@ -1106,20 +1106,20 @@
       <c r="G10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="4">
         <v>-1</v>
       </c>
-      <c r="B11" s="34">
+      <c r="B11" s="51">
         <f>A11-1</f>
         <v>-2</v>
       </c>
-      <c r="C11" s="35"/>
+      <c r="C11" s="41"/>
       <c r="D11" s="4">
         <f>B11-1</f>
         <v>-3</v>
@@ -1154,11 +1154,11 @@
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="38"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="54"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -1170,8 +1170,8 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="6"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="40"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="56"/>
       <c r="D13" s="6"/>
       <c r="E13" s="7"/>
       <c r="F13" s="6"/>
@@ -1182,11 +1182,11 @@
       <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="55"/>
-      <c r="C14" s="56"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="48"/>
       <c r="D14" s="10"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -1200,8 +1200,8 @@
       <c r="A15" s="13">
         <v>1</v>
       </c>
-      <c r="B15" s="57"/>
-      <c r="C15" s="58"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
@@ -1212,17 +1212,17 @@
       <c r="K15" s="16"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="60" t="s">
+      <c r="A16" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="61"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="61"/>
-      <c r="H16" s="61"/>
-      <c r="I16" s="47"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="38"/>
       <c r="J16" s="17">
         <f>SUM(J12:J13)</f>
         <v>0</v>
@@ -1230,14 +1230,14 @@
       <c r="K16" s="18"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="35"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="41"/>
       <c r="G17" s="19" t="e">
         <f>AVERAGE(G13:G15)</f>
         <v>#DIV/0!</v>
@@ -1249,26 +1249,26 @@
       <c r="I17" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="51"/>
-      <c r="K17" s="52"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="44"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="53" t="e">
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="45" t="e">
         <f>AVERAGE(G17:H17)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H18" s="35"/>
+      <c r="H18" s="41"/>
       <c r="I18" s="17"/>
-      <c r="J18" s="44"/>
-      <c r="K18" s="44"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="43"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="21"/>
@@ -1335,10 +1335,10 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="59" t="s">
+      <c r="G23" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="H23" s="42"/>
+      <c r="H23" s="35"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -1363,10 +1363,10 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="59" t="s">
+      <c r="G25" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="H25" s="59"/>
+      <c r="H25" s="34"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -1378,27 +1378,16 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="59" t="s">
+      <c r="G26" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="H26" s="59"/>
+      <c r="H26" s="34"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="A16:I16"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="B15:C15"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="B13:C13"/>
@@ -1411,6 +1400,17 @@
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="K9:K10"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="A16:I16"/>
+    <mergeCell ref="A17:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -1421,7 +1421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D651DB4-1B97-40CF-840B-915296A88124}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -1446,16 +1446,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="19.5" thickTop="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1"/>
@@ -1528,48 +1528,48 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1">
-      <c r="A9" s="64" t="s">
+      <c r="A9" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="64" t="s">
+      <c r="C9" s="54"/>
+      <c r="D9" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="66" t="s">
+      <c r="E9" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="66" t="s">
+      <c r="F9" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="66" t="s">
+      <c r="G9" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="64" t="s">
+      <c r="H9" s="63" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="44"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="4">
         <v>-1</v>
       </c>
-      <c r="B11" s="34">
+      <c r="B11" s="51">
         <f>A11-1</f>
         <v>-2</v>
       </c>
-      <c r="C11" s="35"/>
+      <c r="C11" s="41"/>
       <c r="D11" s="4">
         <f>B11-1</f>
         <v>-3</v>
@@ -1592,11 +1592,11 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="38"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="54"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -1607,8 +1607,8 @@
       <c r="A13" s="6">
         <v>1</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="40"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="56"/>
       <c r="D13" s="6"/>
       <c r="E13" s="7"/>
       <c r="F13" s="6"/>
@@ -1616,11 +1616,11 @@
       <c r="H13" s="25"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="55"/>
-      <c r="C14" s="56"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="48"/>
       <c r="D14" s="10"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -1631,8 +1631,8 @@
       <c r="A15" s="13">
         <v>1</v>
       </c>
-      <c r="B15" s="57"/>
-      <c r="C15" s="58"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
@@ -1640,14 +1640,14 @@
       <c r="H15" s="27"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="62" t="s">
+      <c r="A16" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="35"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="41"/>
       <c r="G16" s="28">
         <f>SUM(G12:G15)</f>
         <v>0</v>
@@ -1757,8 +1757,8 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="42"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="35"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="21"/>
@@ -1767,11 +1767,16 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="59"/>
-      <c r="H26" s="42"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A14:C14"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="B13:C13"/>
@@ -1783,12 +1788,8 @@
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="H9:H10"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A14:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="57" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Penambahan Link utk KHI
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\app\khi\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp82\htdocs\app\khi\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BA76D7-DB6C-4F41-B652-749CA42997AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0A8BA5-3F73-4C1B-8F4B-FD3588F51BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="630" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CKP_R" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t>CKP-R</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>NIP. 197612291999011001</t>
+  </si>
+  <si>
+    <t>Link</t>
   </si>
 </sst>
 </file>
@@ -574,24 +577,42 @@
     <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -609,30 +630,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -643,9 +649,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -927,10 +930,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -943,9 +946,10 @@
     <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21.75" thickTop="1" thickBot="1">
+    <row r="1" spans="1:12" ht="21.75" thickTop="1" thickBot="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -960,22 +964,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="19.5" thickTop="1">
-      <c r="A2" s="57" t="s">
+    <row r="2" spans="1:12" ht="19.5" thickTop="1">
+      <c r="A2" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -988,7 +992,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1005,7 +1009,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1020,7 +1024,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1035,7 +1039,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1050,7 +1054,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1063,40 +1067,43 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="58" t="s">
+    <row r="9" spans="1:12">
+      <c r="A9" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="58" t="s">
+      <c r="C9" s="38"/>
+      <c r="D9" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="40"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="58" t="s">
+      <c r="F9" s="49"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="61" t="s">
+      <c r="I9" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="61" t="s">
+      <c r="J9" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="58" t="s">
+      <c r="K9" s="43" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="43"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="43"/>
+      <c r="L9" s="43" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="44"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="44"/>
       <c r="E10" s="3" t="s">
         <v>13</v>
       </c>
@@ -1106,26 +1113,27 @@
       <c r="G10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43"/>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="44"/>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="4">
         <v>-1</v>
       </c>
-      <c r="B11" s="51">
+      <c r="B11" s="34">
         <f>A11-1</f>
         <v>-2</v>
       </c>
-      <c r="C11" s="41"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="4">
         <f>B11-1</f>
         <v>-3</v>
       </c>
       <c r="E11" s="4">
-        <f t="shared" ref="E11:K11" si="0">D11-1</f>
+        <f t="shared" ref="E11:L11" si="0">D11-1</f>
         <v>-4</v>
       </c>
       <c r="F11" s="4">
@@ -1152,13 +1160,17 @@
         <f t="shared" si="0"/>
         <v>-10</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="52" t="s">
+      <c r="L11" s="4">
+        <f t="shared" si="0"/>
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="53"/>
-      <c r="C12" s="54"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -1167,11 +1179,12 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="6"/>
-      <c r="B13" s="55"/>
-      <c r="C13" s="56"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="40"/>
       <c r="D13" s="6"/>
       <c r="E13" s="7"/>
       <c r="F13" s="6"/>
@@ -1180,13 +1193,14 @@
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="9"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="46" t="s">
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="47"/>
-      <c r="C14" s="48"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="56"/>
       <c r="D14" s="10"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -1195,13 +1209,14 @@
       <c r="I14" s="10"/>
       <c r="J14" s="11"/>
       <c r="K14" s="12"/>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="L14" s="12"/>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="13">
         <v>1</v>
       </c>
-      <c r="B15" s="49"/>
-      <c r="C15" s="50"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="58"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
@@ -1210,34 +1225,36 @@
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
       <c r="K15" s="16"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="36" t="s">
+      <c r="L15" s="16"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="38"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="47"/>
       <c r="J16" s="17">
         <f>SUM(J12:J13)</f>
         <v>0</v>
       </c>
       <c r="K16" s="18"/>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="39" t="s">
+      <c r="L16" s="18"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="41"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="35"/>
       <c r="G17" s="19" t="e">
         <f>AVERAGE(G13:G15)</f>
         <v>#DIV/0!</v>
@@ -1249,28 +1266,30 @@
       <c r="I17" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="42"/>
-      <c r="K17" s="44"/>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="39" t="s">
+      <c r="J17" s="51"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="45" t="e">
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="53" t="e">
         <f>AVERAGE(G17:H17)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H18" s="41"/>
+      <c r="H18" s="35"/>
       <c r="I18" s="17"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="43"/>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="J18" s="44"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="44"/>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="21"/>
       <c r="B19" s="21"/>
       <c r="C19" s="21"/>
@@ -1283,7 +1302,7 @@
       <c r="J19" s="21"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:12">
       <c r="A20" s="21"/>
       <c r="B20" s="22" t="s">
         <v>22</v>
@@ -1298,7 +1317,7 @@
       <c r="J20" s="21"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:12">
       <c r="A21" s="21"/>
       <c r="B21" s="21" t="s">
         <v>23</v>
@@ -1313,7 +1332,7 @@
       <c r="J21" s="21"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:12">
       <c r="A22" s="21"/>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
@@ -1326,7 +1345,7 @@
       <c r="J22" s="21"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:12">
       <c r="A23" s="21"/>
       <c r="B23" s="1"/>
       <c r="C23" s="24" t="s">
@@ -1335,15 +1354,15 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="34" t="s">
+      <c r="G23" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="H23" s="35"/>
+      <c r="H23" s="42"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" ht="55.9" customHeight="1">
+    <row r="24" spans="1:12" ht="55.9" customHeight="1">
       <c r="A24" s="21"/>
       <c r="B24" s="1"/>
       <c r="C24" s="24"/>
@@ -1356,38 +1375,51 @@
       <c r="J24" s="21"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:12">
       <c r="A25" s="21"/>
       <c r="B25" s="1"/>
       <c r="C25" s="24"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="34" t="s">
+      <c r="G25" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="H25" s="34"/>
+      <c r="H25" s="59"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:12">
       <c r="A26" s="21"/>
       <c r="B26" s="1"/>
       <c r="C26" s="24"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="34" t="s">
+      <c r="G26" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="H26" s="34"/>
+      <c r="H26" s="59"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="25">
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="A16:I16"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="B15:C15"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="B13:C13"/>
@@ -1400,17 +1432,6 @@
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="K9:K10"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="A16:I16"/>
-    <mergeCell ref="A17:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -1421,7 +1442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D651DB4-1B97-40CF-840B-915296A88124}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -1446,16 +1467,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="19.5" thickTop="1">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1"/>
@@ -1528,48 +1549,48 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="63" t="s">
+      <c r="C9" s="38"/>
+      <c r="D9" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="65" t="s">
+      <c r="E9" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="65" t="s">
+      <c r="F9" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="65" t="s">
+      <c r="G9" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="63" t="s">
+      <c r="H9" s="64" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="43"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
+      <c r="A10" s="44"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="4">
         <v>-1</v>
       </c>
-      <c r="B11" s="51">
+      <c r="B11" s="34">
         <f>A11-1</f>
         <v>-2</v>
       </c>
-      <c r="C11" s="41"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="4">
         <f>B11-1</f>
         <v>-3</v>
@@ -1592,11 +1613,11 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="52" t="s">
+      <c r="A12" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="53"/>
-      <c r="C12" s="54"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -1607,8 +1628,8 @@
       <c r="A13" s="6">
         <v>1</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="56"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="40"/>
       <c r="D13" s="6"/>
       <c r="E13" s="7"/>
       <c r="F13" s="6"/>
@@ -1616,11 +1637,11 @@
       <c r="H13" s="25"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="47"/>
-      <c r="C14" s="48"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="56"/>
       <c r="D14" s="10"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -1631,8 +1652,8 @@
       <c r="A15" s="13">
         <v>1</v>
       </c>
-      <c r="B15" s="49"/>
-      <c r="C15" s="50"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="58"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
@@ -1640,14 +1661,14 @@
       <c r="H15" s="27"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="66" t="s">
+      <c r="A16" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="41"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="35"/>
       <c r="G16" s="28">
         <f>SUM(G12:G15)</f>
         <v>0</v>
@@ -1757,8 +1778,8 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="35"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="42"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="21"/>
@@ -1767,16 +1788,11 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="35"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A14:C14"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="B13:C13"/>
@@ -1788,6 +1804,11 @@
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="H9:H10"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A14:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="57" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>